<commit_message>
architech pr2-pr4 done, kursovaya code done
</commit_message>
<xml_diff>
--- a/Achitech/tables/PR_4.xlsx
+++ b/Achitech/tables/PR_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Achitech\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938D42AA-3B0E-44B5-BF78-74CD6541E054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA57135A-0460-41F7-A0ED-B3FAA8BA60A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21857" yWindow="-5169" windowWidth="18652" windowHeight="15643" activeTab="1" xr2:uid="{C55A181E-0720-4E4C-8F08-0B75C3FD5C29}"/>
+    <workbookView xWindow="20655" yWindow="5985" windowWidth="17010" windowHeight="15000" xr2:uid="{C55A181E-0720-4E4C-8F08-0B75C3FD5C29}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -217,8 +217,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -226,11 +229,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -668,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A700B0B4-4A28-4133-822F-0BD1DB3D8B14}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +690,7 @@
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -728,7 +728,7 @@
       <c r="E2" s="4">
         <v>0</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="7">
         <v>0</v>
       </c>
     </row>
@@ -748,7 +748,7 @@
       <c r="E3" s="4">
         <v>1</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="7">
         <v>1</v>
       </c>
       <c r="H3" s="3">
@@ -769,7 +769,7 @@
       <c r="M3" s="4">
         <v>0</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -789,7 +789,7 @@
       <c r="E4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="7">
         <v>0</v>
       </c>
       <c r="H4" s="3">
@@ -810,7 +810,7 @@
       <c r="M4" s="4">
         <v>1</v>
       </c>
-      <c r="N4" s="7"/>
+      <c r="N4" s="8"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
@@ -828,7 +828,7 @@
       <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="7">
         <v>0</v>
       </c>
       <c r="H5" s="3">
@@ -849,7 +849,7 @@
       <c r="M5" s="4">
         <v>0</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="8">
         <v>0</v>
       </c>
     </row>
@@ -869,7 +869,7 @@
       <c r="E6" s="4">
         <v>0</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="7">
         <v>0</v>
       </c>
       <c r="H6" s="3">
@@ -890,7 +890,7 @@
       <c r="M6" s="4">
         <v>0</v>
       </c>
-      <c r="N6" s="8"/>
+      <c r="N6" s="9"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
@@ -908,7 +908,7 @@
       <c r="E7" s="4">
         <v>1</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="7">
         <v>1</v>
       </c>
     </row>
@@ -928,7 +928,7 @@
       <c r="E8" s="4">
         <v>0</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="7">
         <v>1</v>
       </c>
       <c r="H8" s="3">
@@ -949,7 +949,7 @@
       <c r="M8" s="4">
         <v>0</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="N8" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -969,7 +969,7 @@
       <c r="E9" s="4">
         <v>1</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="7">
         <v>1</v>
       </c>
       <c r="H9" s="3">
@@ -990,7 +990,7 @@
       <c r="M9" s="4">
         <v>1</v>
       </c>
-      <c r="N9" s="7"/>
+      <c r="N9" s="8"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
@@ -1008,7 +1008,7 @@
       <c r="E10" s="4">
         <v>0</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="7">
         <v>1</v>
       </c>
       <c r="H10" s="3">
@@ -1029,7 +1029,7 @@
       <c r="M10" s="4">
         <v>1</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1049,7 +1049,7 @@
       <c r="E11" s="4">
         <v>1</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="7">
         <v>0</v>
       </c>
       <c r="H11" s="3">
@@ -1070,7 +1070,7 @@
       <c r="M11" s="4">
         <v>1</v>
       </c>
-      <c r="N11" s="8"/>
+      <c r="N11" s="9"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
@@ -1088,7 +1088,7 @@
       <c r="E12" s="4">
         <v>0</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
       <c r="E13" s="4">
         <v>1</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="7">
         <v>0</v>
       </c>
       <c r="H13" s="3">
@@ -1129,7 +1129,7 @@
       <c r="M13" s="4">
         <v>1</v>
       </c>
-      <c r="N13" s="6" t="s">
+      <c r="N13" s="10" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       <c r="E14" s="4">
         <v>0</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="7">
         <v>1</v>
       </c>
       <c r="H14" s="3">
@@ -1170,7 +1170,7 @@
       <c r="M14" s="4">
         <v>0</v>
       </c>
-      <c r="N14" s="7"/>
+      <c r="N14" s="8"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
@@ -1188,7 +1188,7 @@
       <c r="E15" s="4">
         <v>1</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="7">
         <v>1</v>
       </c>
       <c r="H15" s="3">
@@ -1209,7 +1209,7 @@
       <c r="M15" s="4">
         <v>0</v>
       </c>
-      <c r="N15" s="7">
+      <c r="N15" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       <c r="E16" s="4">
         <v>0</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="7">
         <v>1</v>
       </c>
       <c r="H16" s="3">
@@ -1250,7 +1250,7 @@
       <c r="M16" s="4">
         <v>0</v>
       </c>
-      <c r="N16" s="8"/>
+      <c r="N16" s="9"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
@@ -1268,7 +1268,7 @@
       <c r="E17" s="4">
         <v>1</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1288,7 +1288,7 @@
       <c r="E18" s="4">
         <v>0</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="7">
         <v>1</v>
       </c>
       <c r="H18" s="3">
@@ -1309,7 +1309,7 @@
       <c r="M18" s="4">
         <v>1</v>
       </c>
-      <c r="N18" s="6">
+      <c r="N18" s="10">
         <v>1</v>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       <c r="E19" s="4">
         <v>1</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="7">
         <v>0</v>
       </c>
       <c r="H19" s="3">
@@ -1350,7 +1350,7 @@
       <c r="M19" s="4">
         <v>1</v>
       </c>
-      <c r="N19" s="7"/>
+      <c r="N19" s="8"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
@@ -1368,7 +1368,7 @@
       <c r="E20" s="4">
         <v>0</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="7">
         <v>0</v>
       </c>
       <c r="H20" s="3">
@@ -1389,7 +1389,7 @@
       <c r="M20" s="4">
         <v>1</v>
       </c>
-      <c r="N20" s="7" t="s">
+      <c r="N20" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1409,7 +1409,7 @@
       <c r="E21" s="4">
         <v>1</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="7">
         <v>1</v>
       </c>
       <c r="H21" s="3">
@@ -1430,7 +1430,7 @@
       <c r="M21" s="4">
         <v>0</v>
       </c>
-      <c r="N21" s="8"/>
+      <c r="N21" s="9"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
@@ -1448,7 +1448,7 @@
       <c r="E22" s="4">
         <v>0</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1468,7 +1468,7 @@
       <c r="E23" s="4">
         <v>1</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="7">
         <v>1</v>
       </c>
       <c r="H23" s="3">
@@ -1489,7 +1489,7 @@
       <c r="M23" s="4">
         <v>1</v>
       </c>
-      <c r="N23" s="6" t="s">
+      <c r="N23" s="10" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1509,7 +1509,7 @@
       <c r="E24" s="4">
         <v>0</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24" s="7">
         <v>0</v>
       </c>
       <c r="H24" s="3">
@@ -1530,7 +1530,7 @@
       <c r="M24" s="4">
         <v>0</v>
       </c>
-      <c r="N24" s="7"/>
+      <c r="N24" s="8"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
@@ -1548,7 +1548,7 @@
       <c r="E25" s="4">
         <v>1</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25" s="7">
         <v>0</v>
       </c>
       <c r="H25" s="3">
@@ -1569,7 +1569,7 @@
       <c r="M25" s="4">
         <v>0</v>
       </c>
-      <c r="N25" s="7" t="s">
+      <c r="N25" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1589,7 +1589,7 @@
       <c r="E26" s="4">
         <v>0</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26" s="7">
         <v>0</v>
       </c>
       <c r="H26" s="3">
@@ -1610,7 +1610,7 @@
       <c r="M26" s="4">
         <v>1</v>
       </c>
-      <c r="N26" s="8"/>
+      <c r="N26" s="9"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
@@ -1628,7 +1628,7 @@
       <c r="E27" s="4">
         <v>1</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F27" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1648,7 +1648,7 @@
       <c r="E28" s="4">
         <v>0</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F28" s="7">
         <v>0</v>
       </c>
       <c r="H28" s="3">
@@ -1669,7 +1669,7 @@
       <c r="M28" s="4">
         <v>1</v>
       </c>
-      <c r="N28" s="6">
+      <c r="N28" s="10">
         <v>1</v>
       </c>
     </row>
@@ -1689,7 +1689,7 @@
       <c r="E29" s="4">
         <v>1</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F29" s="7">
         <v>1</v>
       </c>
       <c r="H29" s="3">
@@ -1710,7 +1710,7 @@
       <c r="M29" s="4">
         <v>1</v>
       </c>
-      <c r="N29" s="7"/>
+      <c r="N29" s="8"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
@@ -1728,7 +1728,7 @@
       <c r="E30" s="4">
         <v>0</v>
       </c>
-      <c r="F30" s="10">
+      <c r="F30" s="7">
         <v>0</v>
       </c>
       <c r="H30" s="3">
@@ -1749,7 +1749,7 @@
       <c r="M30" s="4">
         <v>0</v>
       </c>
-      <c r="N30" s="7">
+      <c r="N30" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1769,7 +1769,7 @@
       <c r="E31" s="4">
         <v>1</v>
       </c>
-      <c r="F31" s="10">
+      <c r="F31" s="7">
         <v>1</v>
       </c>
       <c r="H31" s="3">
@@ -1790,7 +1790,7 @@
       <c r="M31" s="4">
         <v>0</v>
       </c>
-      <c r="N31" s="8"/>
+      <c r="N31" s="9"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
@@ -1808,7 +1808,7 @@
       <c r="E32" s="4">
         <v>0</v>
       </c>
-      <c r="F32" s="10">
+      <c r="F32" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1828,7 +1828,7 @@
       <c r="E33" s="4">
         <v>1</v>
       </c>
-      <c r="F33" s="10">
+      <c r="F33" s="7">
         <v>0</v>
       </c>
       <c r="H33" s="3">
@@ -1849,7 +1849,7 @@
       <c r="M33" s="4">
         <v>0</v>
       </c>
-      <c r="N33" s="6">
+      <c r="N33" s="10">
         <v>0</v>
       </c>
     </row>
@@ -1872,7 +1872,7 @@
       <c r="M34" s="4">
         <v>0</v>
       </c>
-      <c r="N34" s="7"/>
+      <c r="N34" s="8"/>
     </row>
     <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H35" s="3">
@@ -1893,7 +1893,7 @@
       <c r="M35" s="4">
         <v>0</v>
       </c>
-      <c r="N35" s="7" t="s">
+      <c r="N35" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1916,7 +1916,7 @@
       <c r="M36" s="4">
         <v>1</v>
       </c>
-      <c r="N36" s="8"/>
+      <c r="N36" s="9"/>
     </row>
     <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1938,7 +1938,7 @@
       <c r="M38" s="4">
         <v>0</v>
       </c>
-      <c r="N38" s="6" t="s">
+      <c r="N38" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1961,7 +1961,7 @@
       <c r="M39" s="4">
         <v>1</v>
       </c>
-      <c r="N39" s="7"/>
+      <c r="N39" s="8"/>
     </row>
     <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H40" s="3">
@@ -1982,7 +1982,7 @@
       <c r="M40" s="4">
         <v>1</v>
       </c>
-      <c r="N40" s="7" t="s">
+      <c r="N40" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2005,10 +2005,16 @@
       <c r="M41" s="4">
         <v>0</v>
       </c>
-      <c r="N41" s="8"/>
+      <c r="N41" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="N13:N14"/>
     <mergeCell ref="N35:N36"/>
     <mergeCell ref="N38:N39"/>
     <mergeCell ref="N40:N41"/>
@@ -2019,12 +2025,6 @@
     <mergeCell ref="N20:N21"/>
     <mergeCell ref="N23:N24"/>
     <mergeCell ref="N25:N26"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="N15:N16"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="H3:M6">
@@ -2081,8 +2081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD6D34F7-6838-40DA-A6E3-D8DF1B572407}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2103,7 +2103,7 @@
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -2121,7 +2121,7 @@
       <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       <c r="E2" s="4">
         <v>0</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="7">
         <v>0</v>
       </c>
       <c r="H2" s="3">
@@ -2159,7 +2159,7 @@
       <c r="L2" s="4">
         <v>0</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="7">
         <v>0</v>
       </c>
       <c r="N2" s="5">
@@ -2182,7 +2182,7 @@
       <c r="E3" s="4">
         <v>1</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="7">
         <v>1</v>
       </c>
       <c r="H3" s="3">
@@ -2200,7 +2200,7 @@
       <c r="L3" s="4">
         <v>1</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2220,7 +2220,7 @@
       <c r="E4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="7">
         <v>0</v>
       </c>
       <c r="H4" s="3">
@@ -2238,7 +2238,7 @@
       <c r="L4" s="4">
         <v>0</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="7">
         <v>0</v>
       </c>
     </row>
@@ -2258,7 +2258,7 @@
       <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="7">
         <v>0</v>
       </c>
       <c r="H5" s="3">
@@ -2276,7 +2276,7 @@
       <c r="L5" s="4">
         <v>1</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="7">
         <v>0</v>
       </c>
     </row>
@@ -2296,7 +2296,7 @@
       <c r="E6" s="4">
         <v>0</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="7">
         <v>0</v>
       </c>
     </row>
@@ -2316,7 +2316,7 @@
       <c r="E7" s="4">
         <v>1</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="7">
         <v>1</v>
       </c>
       <c r="H7" s="3">
@@ -2334,7 +2334,7 @@
       <c r="L7" s="4">
         <v>0</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="7">
         <v>0</v>
       </c>
       <c r="N7" s="5">
@@ -2357,7 +2357,7 @@
       <c r="E8" s="4">
         <v>0</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="7">
         <v>1</v>
       </c>
       <c r="H8" s="3">
@@ -2375,7 +2375,7 @@
       <c r="L8" s="4">
         <v>1</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2395,7 +2395,7 @@
       <c r="E9" s="4">
         <v>1</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="7">
         <v>1</v>
       </c>
       <c r="H9" s="3">
@@ -2413,7 +2413,7 @@
       <c r="L9" s="4">
         <v>0</v>
       </c>
-      <c r="M9" s="10">
+      <c r="M9" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2433,7 +2433,7 @@
       <c r="E10" s="4">
         <v>0</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="7">
         <v>1</v>
       </c>
       <c r="H10" s="3">
@@ -2451,7 +2451,7 @@
       <c r="L10" s="4">
         <v>1</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2471,7 +2471,7 @@
       <c r="E11" s="4">
         <v>1</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="7">
         <v>0</v>
       </c>
     </row>
@@ -2491,7 +2491,7 @@
       <c r="E12" s="4">
         <v>0</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="7">
         <v>0</v>
       </c>
       <c r="H12" s="3">
@@ -2509,7 +2509,7 @@
       <c r="L12" s="4">
         <v>0</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="7">
         <v>1</v>
       </c>
       <c r="N12" s="5">
@@ -2532,7 +2532,7 @@
       <c r="E13" s="4">
         <v>1</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="7">
         <v>0</v>
       </c>
       <c r="H13" s="3">
@@ -2550,7 +2550,7 @@
       <c r="L13" s="4">
         <v>1</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="7">
         <v>0</v>
       </c>
     </row>
@@ -2570,7 +2570,7 @@
       <c r="E14" s="4">
         <v>0</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="7">
         <v>1</v>
       </c>
       <c r="H14" s="3">
@@ -2588,7 +2588,7 @@
       <c r="L14" s="4">
         <v>0</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="7">
         <v>0</v>
       </c>
     </row>
@@ -2608,7 +2608,7 @@
       <c r="E15" s="4">
         <v>1</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="7">
         <v>1</v>
       </c>
       <c r="H15" s="3">
@@ -2626,7 +2626,7 @@
       <c r="L15" s="4">
         <v>1</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="7">
         <v>0</v>
       </c>
     </row>
@@ -2646,7 +2646,7 @@
       <c r="E16" s="4">
         <v>0</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2666,7 +2666,7 @@
       <c r="E17" s="4">
         <v>1</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="7">
         <v>0</v>
       </c>
       <c r="H17" s="3">
@@ -2684,7 +2684,7 @@
       <c r="L17" s="4">
         <v>0</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17" s="7">
         <v>1</v>
       </c>
       <c r="N17" s="5">
@@ -2707,7 +2707,7 @@
       <c r="E18" s="4">
         <v>0</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="7">
         <v>1</v>
       </c>
       <c r="H18" s="3">
@@ -2725,7 +2725,7 @@
       <c r="L18" s="4">
         <v>1</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2745,7 +2745,7 @@
       <c r="E19" s="4">
         <v>1</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="7">
         <v>0</v>
       </c>
       <c r="H19" s="3">
@@ -2763,7 +2763,7 @@
       <c r="L19" s="4">
         <v>0</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2783,7 +2783,7 @@
       <c r="E20" s="4">
         <v>0</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="7">
         <v>0</v>
       </c>
       <c r="H20" s="3">
@@ -2801,7 +2801,7 @@
       <c r="L20" s="4">
         <v>1</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="7">
         <v>0</v>
       </c>
     </row>
@@ -2821,7 +2821,7 @@
       <c r="E21" s="4">
         <v>1</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2841,7 +2841,7 @@
       <c r="E22" s="4">
         <v>0</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="7">
         <v>1</v>
       </c>
       <c r="H22" s="3">
@@ -2859,7 +2859,7 @@
       <c r="L22" s="4">
         <v>0</v>
       </c>
-      <c r="M22" s="10">
+      <c r="M22" s="7">
         <v>1</v>
       </c>
       <c r="N22" s="5">
@@ -2882,7 +2882,7 @@
       <c r="E23" s="4">
         <v>1</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="7">
         <v>1</v>
       </c>
       <c r="H23" s="3">
@@ -2900,7 +2900,7 @@
       <c r="L23" s="4">
         <v>1</v>
       </c>
-      <c r="M23" s="10">
+      <c r="M23" s="7">
         <v>0</v>
       </c>
     </row>
@@ -2920,7 +2920,7 @@
       <c r="E24" s="4">
         <v>0</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24" s="7">
         <v>0</v>
       </c>
       <c r="H24" s="3">
@@ -2938,7 +2938,7 @@
       <c r="L24" s="4">
         <v>0</v>
       </c>
-      <c r="M24" s="10">
+      <c r="M24" s="7">
         <v>0</v>
       </c>
     </row>
@@ -2958,7 +2958,7 @@
       <c r="E25" s="4">
         <v>1</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25" s="7">
         <v>0</v>
       </c>
       <c r="H25" s="3">
@@ -2976,7 +2976,7 @@
       <c r="L25" s="4">
         <v>1</v>
       </c>
-      <c r="M25" s="10">
+      <c r="M25" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       <c r="E26" s="4">
         <v>0</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26" s="7">
         <v>0</v>
       </c>
     </row>
@@ -3016,7 +3016,7 @@
       <c r="E27" s="4">
         <v>1</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F27" s="7">
         <v>0</v>
       </c>
       <c r="H27" s="3">
@@ -3034,7 +3034,7 @@
       <c r="L27" s="4">
         <v>0</v>
       </c>
-      <c r="M27" s="10">
+      <c r="M27" s="7">
         <v>1</v>
       </c>
       <c r="N27" s="5">
@@ -3057,7 +3057,7 @@
       <c r="E28" s="4">
         <v>0</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F28" s="7">
         <v>0</v>
       </c>
       <c r="H28" s="3">
@@ -3075,7 +3075,7 @@
       <c r="L28" s="4">
         <v>1</v>
       </c>
-      <c r="M28" s="10">
+      <c r="M28" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3095,7 +3095,7 @@
       <c r="E29" s="4">
         <v>1</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F29" s="7">
         <v>1</v>
       </c>
       <c r="H29" s="3">
@@ -3113,7 +3113,7 @@
       <c r="L29" s="4">
         <v>0</v>
       </c>
-      <c r="M29" s="10">
+      <c r="M29" s="7">
         <v>0</v>
       </c>
     </row>
@@ -3133,7 +3133,7 @@
       <c r="E30" s="4">
         <v>0</v>
       </c>
-      <c r="F30" s="10">
+      <c r="F30" s="7">
         <v>0</v>
       </c>
       <c r="H30" s="3">
@@ -3151,7 +3151,7 @@
       <c r="L30" s="4">
         <v>1</v>
       </c>
-      <c r="M30" s="10">
+      <c r="M30" s="7">
         <v>0</v>
       </c>
     </row>
@@ -3171,7 +3171,7 @@
       <c r="E31" s="4">
         <v>1</v>
       </c>
-      <c r="F31" s="10">
+      <c r="F31" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3191,7 +3191,7 @@
       <c r="E32" s="4">
         <v>0</v>
       </c>
-      <c r="F32" s="10">
+      <c r="F32" s="7">
         <v>1</v>
       </c>
       <c r="H32" s="3">
@@ -3209,7 +3209,7 @@
       <c r="L32" s="4">
         <v>0</v>
       </c>
-      <c r="M32" s="10">
+      <c r="M32" s="7">
         <v>0</v>
       </c>
       <c r="N32" s="5">
@@ -3232,7 +3232,7 @@
       <c r="E33" s="4">
         <v>1</v>
       </c>
-      <c r="F33" s="10">
+      <c r="F33" s="7">
         <v>0</v>
       </c>
       <c r="H33" s="3">
@@ -3250,7 +3250,7 @@
       <c r="L33" s="4">
         <v>1</v>
       </c>
-      <c r="M33" s="10">
+      <c r="M33" s="7">
         <v>0</v>
       </c>
     </row>
@@ -3270,7 +3270,7 @@
       <c r="L34" s="4">
         <v>0</v>
       </c>
-      <c r="M34" s="10">
+      <c r="M34" s="7">
         <v>0</v>
       </c>
     </row>
@@ -3290,7 +3290,7 @@
       <c r="L35" s="4">
         <v>1</v>
       </c>
-      <c r="M35" s="10">
+      <c r="M35" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3310,7 +3310,7 @@
       <c r="L37" s="4">
         <v>0</v>
       </c>
-      <c r="M37" s="10">
+      <c r="M37" s="7">
         <v>0</v>
       </c>
       <c r="N37" s="5">
@@ -3333,7 +3333,7 @@
       <c r="L38" s="4">
         <v>1</v>
       </c>
-      <c r="M38" s="10">
+      <c r="M38" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3353,7 +3353,7 @@
       <c r="L39" s="4">
         <v>0</v>
       </c>
-      <c r="M39" s="10">
+      <c r="M39" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3373,7 +3373,7 @@
       <c r="L40" s="4">
         <v>1</v>
       </c>
-      <c r="M40" s="10">
+      <c r="M40" s="7">
         <v>0</v>
       </c>
     </row>

</xml_diff>